<commit_message>
Added Benchmark Datasets and ability to display Gantt Chart
</commit_message>
<xml_diff>
--- a/data/Machines_Data_Testing.xlsx
+++ b/data/Machines_Data_Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79ADABB-10BB-4851-B2AF-41EDE217D7EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DD17C0-B26F-4592-8B89-FF9EB180A7C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3673E1-565D-41DE-9737-D9BBE2EAEAF2}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,13 +547,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -562,16 +562,16 @@
       </c>
       <c r="B3">
         <f>C2</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -580,17 +580,17 @@
       </c>
       <c r="B4">
         <f>D2</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>D3</f>
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -599,15 +599,15 @@
       </c>
       <c r="B5">
         <f>E2</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f>E3</f>
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f>E4</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>

</xml_diff>